<commit_message>
HD5 hash check added
this adds a way to create a HD5 hash for each of the files in the
repository, as well as a way to compare the current hash with the one on
GitHub.
</commit_message>
<xml_diff>
--- a/Project Database.xlsx
+++ b/Project Database.xlsx
@@ -458,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="A6:D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updates to various files
various updates to several files so that they work better together.
</commit_message>
<xml_diff>
--- a/Project Database.xlsx
+++ b/Project Database.xlsx
@@ -456,10 +456,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +475,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -546,7 +549,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Location " prompt="Please select where this project is located on the LRC network._x000a_DO NOT CHOSE A LOCAL DIRECTORY, the value here will be used in various programs through out the network._x000a_" sqref="D2:D4"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="86" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>